<commit_message>
Actualizar .gitignore para ignorar .DS_Store
</commit_message>
<xml_diff>
--- a/Large Images/reports/report.xlsx
+++ b/Large Images/reports/report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1920,10 +1920,8 @@
           <t>segmentation</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>21691136843814</t>
-        </is>
+      <c r="C35" t="n">
+        <v>21691136843814</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1952,6 +1950,626 @@
       <c r="J35" t="inlineStr">
         <is>
           <t>2025-02-28 19:22:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>21691136843814</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>9.30 minutes</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>SegFormer-[14M]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>73.19%</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>39.49%</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>56.72%</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>2025-03-09 16:09:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>21691136843814</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>9.49 minutes</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>SegFormer-[14M]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>72.43%</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>45.77%</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>56.86%</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>2025-03-09 16:59:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>21691136843814</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>9.41 minutes</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>SegFormer-[14M]</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>73.27%</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>39.25%</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>56.69%</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>2025-03-10 00:45:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>103610396583974</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>5.50 minutes</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>RepPoints-[37M]</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>{'height': 2000, 'width': 2000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>85.25%</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>2025-03-10 00:59:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>21691136843814</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>9.26 minutes</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>SegFormer-[14M]</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>73.77%</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>43.71%</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>56.74%</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>2025-03-10 01:11:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>21691136843814</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>10.47 minutes</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>FastVit-[14M]</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>72.00%</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>52.28%</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>56.32%</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>2025-03-10 01:22:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>1938830</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>6.44 minutes</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>FastVit-[14M]</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>{'height': 2048, 'width': 2048, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>19.41%</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>6.78%</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>24.80%</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>2025-03-10 01:35:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>segmentation</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>1938830</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>6.05 minutes</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>SegFormer-[14M]</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>{'height': 2048, 'width': 2048, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>30.07%</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>11.42%</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>45.54%</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>2025-03-10 01:44:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>102004060440613</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>11.19 minutes</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>RtmDet-[9M]</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>{'height': 3040, 'width': 4056, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>70.80%</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>68.75%</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>66.67%</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>2025-03-10 01:56:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>6464689526794</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>8.38 minutes</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>RtmDet-[9M]</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>77.68%</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>76.92%</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>76.92%</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>2025-03-10 02:08:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>6464689526794</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>10.03 minutes</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>RepPoints-[20M]</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>76.56%</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>80.00%</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>73.08%</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>2025-03-10 02:24:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Large Images</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>object-detection</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>6464689526794</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>12.82 minutes</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>RepPoints-[37M]</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>{'height': 6000, 'width': 6000, 'paddingValue': 0}</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>73.38%</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>71.43%</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>78.26%</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>2025-03-10 02:37:41</t>
         </is>
       </c>
     </row>

</xml_diff>